<commit_message>
fixes in conversion script
</commit_message>
<xml_diff>
--- a/HSE MNIS/Converted.xlsx
+++ b/HSE MNIS/Converted.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,16 @@
           <t>rate</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>CRNCY_ADJ_MKT_CAP_USD</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>BS_TOT_ASSET_USD</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -464,10 +474,14 @@
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>303628067.7417991</v>
+        <v>1967874298.9</v>
       </c>
       <c r="E2" t="n">
         <v>6.481200218200684</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="n">
+        <v>303628067.7417991</v>
       </c>
     </row>
     <row r="3">
@@ -482,6 +496,8 @@
       <c r="E3" t="n">
         <v>6.945300102233887</v>
       </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -492,10 +508,14 @@
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>328666684.9013267</v>
+        <v>2146719318.6</v>
       </c>
       <c r="E4" t="n">
         <v>6.531599998474121</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="n">
+        <v>328666684.9013267</v>
       </c>
     </row>
     <row r="5">
@@ -507,10 +527,14 @@
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>335293119.3546522</v>
+        <v>2305877882.89</v>
       </c>
       <c r="E5" t="n">
         <v>6.877200126647949</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="n">
+        <v>335293119.3546522</v>
       </c>
     </row>
     <row r="6">
@@ -522,10 +546,14 @@
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>537018747.0202146</v>
+        <v>3751451931.12</v>
       </c>
       <c r="E6" t="n">
         <v>6.985700130462646</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>537018747.0202146</v>
       </c>
     </row>
     <row r="7">
@@ -537,10 +565,14 @@
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>700895964.8203815</v>
+        <v>4571383737.15</v>
       </c>
       <c r="E7" t="n">
         <v>6.522200107574463</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="n">
+        <v>700895964.8203815</v>
       </c>
     </row>
     <row r="8">
@@ -551,13 +583,19 @@
         <v>2021</v>
       </c>
       <c r="C8" t="n">
-        <v>1822354298.933797</v>
+        <v>11612223603</v>
       </c>
       <c r="D8" t="n">
-        <v>1008819182.542052</v>
+        <v>6428296588.39</v>
       </c>
       <c r="E8" t="n">
         <v>6.372099876403809</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1822354298.933797</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1008819182.542052</v>
       </c>
     </row>
     <row r="9">
@@ -568,13 +606,19 @@
         <v>2022</v>
       </c>
       <c r="C9" t="n">
-        <v>1112184973.304447</v>
+        <v>7744255139.25</v>
       </c>
       <c r="D9" t="n">
-        <v>999743962.6382524</v>
+        <v>6961317142.77</v>
       </c>
       <c r="E9" t="n">
         <v>6.963099956512451</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1112184973.304447</v>
+      </c>
+      <c r="G9" t="n">
+        <v>999743962.6382524</v>
       </c>
     </row>
     <row r="10">
@@ -585,13 +629,19 @@
         <v>2023</v>
       </c>
       <c r="C10" t="n">
-        <v>1330773452.550222</v>
+        <v>9457806759.75</v>
       </c>
       <c r="D10" t="n">
-        <v>884206657.3938882</v>
+        <v>6284056602.79</v>
       </c>
       <c r="E10" t="n">
         <v>7.10699987411499</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1330773452.550222</v>
+      </c>
+      <c r="G10" t="n">
+        <v>884206657.3938882</v>
       </c>
     </row>
     <row r="11">
@@ -602,13 +652,19 @@
         <v>2024</v>
       </c>
       <c r="C11" t="n">
-        <v>4474767316.753379</v>
+        <v>32657299330.5</v>
       </c>
       <c r="D11" t="n">
-        <v>1053089113.384868</v>
+        <v>7685549652.77</v>
       </c>
       <c r="E11" t="n">
         <v>7.298099994659424</v>
+      </c>
+      <c r="F11" t="n">
+        <v>4474767316.753379</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1053089113.384868</v>
       </c>
     </row>
     <row r="12">
@@ -619,13 +675,19 @@
         <v>2015</v>
       </c>
       <c r="C12" t="n">
-        <v>6603760134.366325</v>
+        <v>42800291623.8</v>
       </c>
       <c r="D12" t="n">
-        <v>1774898234.79695</v>
+        <v>11503470826.65</v>
       </c>
       <c r="E12" t="n">
         <v>6.481200218200684</v>
+      </c>
+      <c r="F12" t="n">
+        <v>6603760134.366325</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1774898234.79695</v>
       </c>
     </row>
     <row r="13">
@@ -636,13 +698,19 @@
         <v>2016</v>
       </c>
       <c r="C13" t="n">
-        <v>5710904847.386291</v>
+        <v>39663948020.4</v>
       </c>
       <c r="D13" t="n">
-        <v>2212488692.164295</v>
+        <v>15366397939.88</v>
       </c>
       <c r="E13" t="n">
         <v>6.945300102233887</v>
+      </c>
+      <c r="F13" t="n">
+        <v>5710904847.386291</v>
+      </c>
+      <c r="G13" t="n">
+        <v>2212488692.164295</v>
       </c>
     </row>
     <row r="14">
@@ -653,13 +721,19 @@
         <v>2017</v>
       </c>
       <c r="C14" t="n">
-        <v>10247455303.04005</v>
+        <v>66932279041.7</v>
       </c>
       <c r="D14" t="n">
-        <v>3266194893.893352</v>
+        <v>21333478563.97</v>
       </c>
       <c r="E14" t="n">
         <v>6.531599998474121</v>
+      </c>
+      <c r="F14" t="n">
+        <v>10247455303.04005</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3266194893.893352</v>
       </c>
     </row>
     <row r="15">
@@ -670,13 +744,19 @@
         <v>2018</v>
       </c>
       <c r="C15" t="n">
-        <v>4995164701.502448</v>
+        <v>34352747317.8</v>
       </c>
       <c r="D15" t="n">
-        <v>3831588334.334787</v>
+        <v>26350599778.15</v>
       </c>
       <c r="E15" t="n">
         <v>6.877200126647949</v>
+      </c>
+      <c r="F15" t="n">
+        <v>4995164701.502448</v>
+      </c>
+      <c r="G15" t="n">
+        <v>3831588334.334787</v>
       </c>
     </row>
     <row r="16">
@@ -687,13 +767,19 @@
         <v>2019</v>
       </c>
       <c r="C16" t="n">
-        <v>8560182162.935137</v>
+        <v>59798865652.4</v>
       </c>
       <c r="D16" t="n">
-        <v>4232167092.888369</v>
+        <v>29564650212.93</v>
       </c>
       <c r="E16" t="n">
         <v>6.985700130462646</v>
+      </c>
+      <c r="F16" t="n">
+        <v>8560182162.935137</v>
+      </c>
+      <c r="G16" t="n">
+        <v>4232167092.888369</v>
       </c>
     </row>
     <row r="17">
@@ -704,13 +790,19 @@
         <v>2020</v>
       </c>
       <c r="C17" t="n">
-        <v>9135272923.611345</v>
+        <v>59582078045.1</v>
       </c>
       <c r="D17" t="n">
-        <v>5610841966.999891</v>
+        <v>36595034080.75</v>
       </c>
       <c r="E17" t="n">
         <v>6.522200107574463</v>
+      </c>
+      <c r="F17" t="n">
+        <v>9135272923.611345</v>
+      </c>
+      <c r="G17" t="n">
+        <v>5610841966.999891</v>
       </c>
     </row>
     <row r="18">
@@ -721,13 +813,19 @@
         <v>2021</v>
       </c>
       <c r="C18" t="n">
-        <v>11038152279.07183</v>
+        <v>70336208773.2</v>
       </c>
       <c r="D18" t="n">
-        <v>6913870290.249374</v>
+        <v>44055872021.97</v>
       </c>
       <c r="E18" t="n">
         <v>6.372099876403809</v>
+      </c>
+      <c r="F18" t="n">
+        <v>11038152279.07183</v>
+      </c>
+      <c r="G18" t="n">
+        <v>6913870290.249374</v>
       </c>
     </row>
     <row r="19">
@@ -738,13 +836,19 @@
         <v>2022</v>
       </c>
       <c r="C19" t="n">
-        <v>4926692571.83579</v>
+        <v>34305052832.7</v>
       </c>
       <c r="D19" t="n">
-        <v>6642572143.644237</v>
+        <v>46252893804.54</v>
       </c>
       <c r="E19" t="n">
         <v>6.963099956512451</v>
+      </c>
+      <c r="F19" t="n">
+        <v>4926692571.83579</v>
+      </c>
+      <c r="G19" t="n">
+        <v>6642572143.644237</v>
       </c>
     </row>
     <row r="20">
@@ -755,13 +859,19 @@
         <v>2023</v>
       </c>
       <c r="C20" t="n">
-        <v>8552547339.54376</v>
+        <v>60782952865.5</v>
       </c>
       <c r="D20" t="n">
-        <v>7440822871.913333</v>
+        <v>52881927214</v>
       </c>
       <c r="E20" t="n">
         <v>7.10699987411499</v>
+      </c>
+      <c r="F20" t="n">
+        <v>8552547339.54376</v>
+      </c>
+      <c r="G20" t="n">
+        <v>7440822871.913333</v>
       </c>
     </row>
     <row r="21">
@@ -772,13 +882,19 @@
         <v>2024</v>
       </c>
       <c r="C21" t="n">
-        <v>7225178576.148123</v>
+        <v>52730075728</v>
       </c>
       <c r="D21" t="n">
-        <v>7225978284.815348</v>
+        <v>52735912081.82</v>
       </c>
       <c r="E21" t="n">
         <v>7.298099994659424</v>
+      </c>
+      <c r="F21" t="n">
+        <v>7225178576.148123</v>
+      </c>
+      <c r="G21" t="n">
+        <v>7225978284.815348</v>
       </c>
     </row>
     <row r="22">
@@ -790,10 +906,14 @@
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="n">
-        <v>413447130.3455461</v>
+        <v>2679633631.41</v>
       </c>
       <c r="E22" t="n">
         <v>6.481200218200684</v>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="n">
+        <v>413447130.3455461</v>
       </c>
     </row>
     <row r="23">
@@ -805,10 +925,14 @@
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
-        <v>624431444.6650176</v>
+        <v>4336863776.47</v>
       </c>
       <c r="E23" t="n">
         <v>6.945300102233887</v>
+      </c>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="n">
+        <v>624431444.6650176</v>
       </c>
     </row>
     <row r="24">
@@ -819,13 +943,19 @@
         <v>2017</v>
       </c>
       <c r="C24" t="n">
-        <v>3358772736.408396</v>
+        <v>21938160000</v>
       </c>
       <c r="D24" t="n">
-        <v>731428233.4766475</v>
+        <v>4777396648.66</v>
       </c>
       <c r="E24" t="n">
         <v>6.531599998474121</v>
+      </c>
+      <c r="F24" t="n">
+        <v>3358772736.408396</v>
+      </c>
+      <c r="G24" t="n">
+        <v>731428233.4766475</v>
       </c>
     </row>
     <row r="25">
@@ -836,13 +966,19 @@
         <v>2018</v>
       </c>
       <c r="C25" t="n">
-        <v>2987537024.02643</v>
+        <v>20545890000</v>
       </c>
       <c r="D25" t="n">
-        <v>1115295374.614687</v>
+        <v>7670109491.55</v>
       </c>
       <c r="E25" t="n">
         <v>6.877200126647949</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2987537024.02643</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1115295374.614687</v>
       </c>
     </row>
     <row r="26">
@@ -853,13 +989,19 @@
         <v>2019</v>
       </c>
       <c r="C26" t="n">
-        <v>3778565277.243279</v>
+        <v>26395923950.2</v>
       </c>
       <c r="D26" t="n">
-        <v>1262583876.948619</v>
+        <v>8820032353.92</v>
       </c>
       <c r="E26" t="n">
         <v>6.985700130462646</v>
+      </c>
+      <c r="F26" t="n">
+        <v>3778565277.243279</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1262583876.948619</v>
       </c>
     </row>
     <row r="27">
@@ -870,13 +1012,19 @@
         <v>2020</v>
       </c>
       <c r="C27" t="n">
-        <v>3945376245.695972</v>
+        <v>25732533374.1</v>
       </c>
       <c r="D27" t="n">
-        <v>1856046676.68682</v>
+        <v>12105507834.35</v>
       </c>
       <c r="E27" t="n">
         <v>6.522200107574463</v>
+      </c>
+      <c r="F27" t="n">
+        <v>3945376245.695972</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1856046676.68682</v>
       </c>
     </row>
     <row r="28">
@@ -887,13 +1035,19 @@
         <v>2021</v>
       </c>
       <c r="C28" t="n">
-        <v>4615159074.346931</v>
+        <v>29408254567.23</v>
       </c>
       <c r="D28" t="n">
-        <v>2250722890.697066</v>
+        <v>14341831053.63</v>
       </c>
       <c r="E28" t="n">
         <v>6.372099876403809</v>
+      </c>
+      <c r="F28" t="n">
+        <v>4615159074.346931</v>
+      </c>
+      <c r="G28" t="n">
+        <v>2250722890.697066</v>
       </c>
     </row>
     <row r="29">
@@ -904,13 +1058,19 @@
         <v>2022</v>
       </c>
       <c r="C29" t="n">
-        <v>2462745923.312717</v>
+        <v>17148346031.52</v>
       </c>
       <c r="D29" t="n">
-        <v>2224808924.285374</v>
+        <v>15491566923.94</v>
       </c>
       <c r="E29" t="n">
         <v>6.963099956512451</v>
+      </c>
+      <c r="F29" t="n">
+        <v>2462745923.312717</v>
+      </c>
+      <c r="G29" t="n">
+        <v>2224808924.285374</v>
       </c>
     </row>
     <row r="30">
@@ -921,13 +1081,19 @@
         <v>2023</v>
       </c>
       <c r="C30" t="n">
-        <v>2672385278.842443</v>
+        <v>18992641840.32</v>
       </c>
       <c r="D30" t="n">
-        <v>2424473392.689581</v>
+        <v>17230732096.64</v>
       </c>
       <c r="E30" t="n">
         <v>7.10699987411499</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2672385278.842443</v>
+      </c>
+      <c r="G30" t="n">
+        <v>2424473392.689581</v>
       </c>
     </row>
     <row r="31">
@@ -938,13 +1104,19 @@
         <v>2024</v>
       </c>
       <c r="C31" t="n">
-        <v>3557323082.045759</v>
+        <v>25961699566.08</v>
       </c>
       <c r="D31" t="n">
-        <v>2636820153.296356</v>
+        <v>19243777146.69</v>
       </c>
       <c r="E31" t="n">
         <v>7.298099994659424</v>
+      </c>
+      <c r="F31" t="n">
+        <v>3557323082.045759</v>
+      </c>
+      <c r="G31" t="n">
+        <v>2636820153.296356</v>
       </c>
     </row>
     <row r="32">
@@ -955,13 +1127,19 @@
         <v>2015</v>
       </c>
       <c r="C32" t="n">
-        <v>2901055966.226564</v>
+        <v>18802324561.32</v>
       </c>
       <c r="D32" t="n">
-        <v>784414304.4884068</v>
+        <v>5083946161.41</v>
       </c>
       <c r="E32" t="n">
         <v>6.481200218200684</v>
+      </c>
+      <c r="F32" t="n">
+        <v>2901055966.226564</v>
+      </c>
+      <c r="G32" t="n">
+        <v>784414304.4884068</v>
       </c>
     </row>
     <row r="33">
@@ -972,13 +1150,19 @@
         <v>2016</v>
       </c>
       <c r="C33" t="n">
-        <v>3379886577.394938</v>
+        <v>23474326591.52</v>
       </c>
       <c r="D33" t="n">
-        <v>1178143790.088805</v>
+        <v>8182562185.75</v>
       </c>
       <c r="E33" t="n">
         <v>6.945300102233887</v>
+      </c>
+      <c r="F33" t="n">
+        <v>3379886577.394938</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1178143790.088805</v>
       </c>
     </row>
     <row r="34">
@@ -989,13 +1173,19 @@
         <v>2017</v>
       </c>
       <c r="C34" t="n">
-        <v>2792544465.092946</v>
+        <v>18239783423.94</v>
       </c>
       <c r="D34" t="n">
-        <v>1543801229.759271</v>
+        <v>10083492109.94</v>
       </c>
       <c r="E34" t="n">
         <v>6.531599998474121</v>
+      </c>
+      <c r="F34" t="n">
+        <v>2792544465.092946</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1543801229.759271</v>
       </c>
     </row>
     <row r="35">
@@ -1006,13 +1196,19 @@
         <v>2018</v>
       </c>
       <c r="C35" t="n">
-        <v>1083544961.401625</v>
+        <v>7451755545.78</v>
       </c>
       <c r="D35" t="n">
-        <v>1426668046.439745</v>
+        <v>9811481669.66</v>
       </c>
       <c r="E35" t="n">
         <v>6.877200126647949</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1083544961.401625</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1426668046.439745</v>
       </c>
     </row>
     <row r="36">
@@ -1023,13 +1219,19 @@
         <v>2019</v>
       </c>
       <c r="C36" t="n">
-        <v>2317078282.589839</v>
+        <v>16186414060.98</v>
       </c>
       <c r="D36" t="n">
-        <v>1380918537.811774</v>
+        <v>9646682809.75</v>
       </c>
       <c r="E36" t="n">
         <v>6.985700130462646</v>
+      </c>
+      <c r="F36" t="n">
+        <v>2317078282.589839</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1380918537.811774</v>
       </c>
     </row>
     <row r="37">
@@ -1040,13 +1242,19 @@
         <v>2020</v>
       </c>
       <c r="C37" t="n">
-        <v>3782636317.896558</v>
+        <v>24671110999.5</v>
       </c>
       <c r="D37" t="n">
-        <v>2088231124.845859</v>
+        <v>13619861267.11</v>
       </c>
       <c r="E37" t="n">
         <v>6.522200107574463</v>
+      </c>
+      <c r="F37" t="n">
+        <v>3782636317.896558</v>
+      </c>
+      <c r="G37" t="n">
+        <v>2088231124.845859</v>
       </c>
     </row>
     <row r="38">
@@ -1057,13 +1265,19 @@
         <v>2021</v>
       </c>
       <c r="C38" t="n">
-        <v>3739487821.538653</v>
+        <v>23828389885.44</v>
       </c>
       <c r="D38" t="n">
-        <v>2664561147.98255</v>
+        <v>16978849761.73</v>
       </c>
       <c r="E38" t="n">
         <v>6.372099876403809</v>
+      </c>
+      <c r="F38" t="n">
+        <v>3739487821.538653</v>
+      </c>
+      <c r="G38" t="n">
+        <v>2664561147.98255</v>
       </c>
     </row>
     <row r="39">
@@ -1074,13 +1288,19 @@
         <v>2022</v>
       </c>
       <c r="C39" t="n">
-        <v>1781766222.482033</v>
+        <v>12406616306.28</v>
       </c>
       <c r="D39" t="n">
-        <v>2524844068.265468</v>
+        <v>17580741621.94</v>
       </c>
       <c r="E39" t="n">
         <v>6.963099956512451</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1781766222.482033</v>
+      </c>
+      <c r="G39" t="n">
+        <v>2524844068.265468</v>
       </c>
     </row>
     <row r="40">
@@ -1091,13 +1311,19 @@
         <v>2023</v>
       </c>
       <c r="C40" t="n">
-        <v>2244147692.416569</v>
+        <v>15949157367.5</v>
       </c>
       <c r="D40" t="n">
-        <v>2613317562.778599</v>
+        <v>18572847589.69</v>
       </c>
       <c r="E40" t="n">
         <v>7.10699987411499</v>
+      </c>
+      <c r="F40" t="n">
+        <v>2244147692.416569</v>
+      </c>
+      <c r="G40" t="n">
+        <v>2613317562.778599</v>
       </c>
     </row>
     <row r="41">
@@ -1108,13 +1334,19 @@
         <v>2024</v>
       </c>
       <c r="C41" t="n">
-        <v>3016792125.1218</v>
+        <v>22016850592.24</v>
       </c>
       <c r="D41" t="n">
-        <v>2763515430.99831</v>
+        <v>20168411952.21</v>
       </c>
       <c r="E41" t="n">
         <v>7.298099994659424</v>
+      </c>
+      <c r="F41" t="n">
+        <v>3016792125.1218</v>
+      </c>
+      <c r="G41" t="n">
+        <v>2763515430.99831</v>
       </c>
     </row>
     <row r="42">
@@ -1125,13 +1357,19 @@
         <v>2015</v>
       </c>
       <c r="C42" t="n">
-        <v>2820773835.787388</v>
+        <v>18282000000</v>
       </c>
       <c r="D42" t="n">
-        <v>514980574.6360067</v>
+        <v>3337692212.7</v>
       </c>
       <c r="E42" t="n">
         <v>6.481200218200684</v>
+      </c>
+      <c r="F42" t="n">
+        <v>2820773835.787388</v>
+      </c>
+      <c r="G42" t="n">
+        <v>514980574.6360067</v>
       </c>
     </row>
     <row r="43">
@@ -1142,13 +1380,19 @@
         <v>2016</v>
       </c>
       <c r="C43" t="n">
-        <v>2047507260.572671</v>
+        <v>14220552386.18</v>
       </c>
       <c r="D43" t="n">
-        <v>584965908.2957772</v>
+        <v>4062763782.69</v>
       </c>
       <c r="E43" t="n">
         <v>6.945300102233887</v>
+      </c>
+      <c r="F43" t="n">
+        <v>2047507260.572671</v>
+      </c>
+      <c r="G43" t="n">
+        <v>584965908.2957772</v>
       </c>
     </row>
     <row r="44">
@@ -1159,13 +1403,19 @@
         <v>2017</v>
       </c>
       <c r="C44" t="n">
-        <v>1606611532.176112</v>
+        <v>10493743881.11</v>
       </c>
       <c r="D44" t="n">
-        <v>631674072.863289</v>
+        <v>4125842373.35</v>
       </c>
       <c r="E44" t="n">
         <v>6.531599998474121</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1606611532.176112</v>
+      </c>
+      <c r="G44" t="n">
+        <v>631674072.863289</v>
       </c>
     </row>
     <row r="45">
@@ -1176,13 +1426,19 @@
         <v>2018</v>
       </c>
       <c r="C45" t="n">
-        <v>1956132905.878814</v>
+        <v>13452717468.05</v>
       </c>
       <c r="D45" t="n">
-        <v>640245575.1547447</v>
+        <v>4403096950.54</v>
       </c>
       <c r="E45" t="n">
         <v>6.877200126647949</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1956132905.878814</v>
+      </c>
+      <c r="G45" t="n">
+        <v>640245575.1547447</v>
       </c>
     </row>
     <row r="46">
@@ -1193,13 +1449,19 @@
         <v>2019</v>
       </c>
       <c r="C46" t="n">
-        <v>2814902529.275572</v>
+        <v>19664064966</v>
       </c>
       <c r="D46" t="n">
-        <v>620171431.1151057</v>
+        <v>4332331647.25</v>
       </c>
       <c r="E46" t="n">
         <v>6.985700130462646</v>
+      </c>
+      <c r="F46" t="n">
+        <v>2814902529.275572</v>
+      </c>
+      <c r="G46" t="n">
+        <v>620171431.1151057</v>
       </c>
     </row>
     <row r="47">
@@ -1210,13 +1472,19 @@
         <v>2020</v>
       </c>
       <c r="C47" t="n">
-        <v>10189791260.66951</v>
+        <v>66459857656.5</v>
       </c>
       <c r="D47" t="n">
-        <v>971872336.8850013</v>
+        <v>6338745860.18</v>
       </c>
       <c r="E47" t="n">
         <v>6.522200107574463</v>
+      </c>
+      <c r="F47" t="n">
+        <v>10189791260.66951</v>
+      </c>
+      <c r="G47" t="n">
+        <v>971872336.8850013</v>
       </c>
     </row>
     <row r="48">
@@ -1227,13 +1495,19 @@
         <v>2021</v>
       </c>
       <c r="C48" t="n">
-        <v>8915456065.243235</v>
+        <v>56810176491.42</v>
       </c>
       <c r="D48" t="n">
-        <v>1453114007.560986</v>
+        <v>9259387587.98</v>
       </c>
       <c r="E48" t="n">
         <v>6.372099876403809</v>
+      </c>
+      <c r="F48" t="n">
+        <v>8915456065.243235</v>
+      </c>
+      <c r="G48" t="n">
+        <v>1453114007.560986</v>
       </c>
     </row>
     <row r="49">
@@ -1244,13 +1518,19 @@
         <v>2022</v>
       </c>
       <c r="C49" t="n">
-        <v>5189785880.956911</v>
+        <v>36136997842</v>
       </c>
       <c r="D49" t="n">
-        <v>1276413890.670551</v>
+        <v>8887797506.620001</v>
       </c>
       <c r="E49" t="n">
         <v>6.963099956512451</v>
+      </c>
+      <c r="F49" t="n">
+        <v>5189785880.956911</v>
+      </c>
+      <c r="G49" t="n">
+        <v>1276413890.670551</v>
       </c>
     </row>
     <row r="50">
@@ -1261,13 +1541,19 @@
         <v>2023</v>
       </c>
       <c r="C50" t="n">
-        <v>4386713682.372519</v>
+        <v>31176373588.4</v>
       </c>
       <c r="D50" t="n">
-        <v>1213243616.863541</v>
+        <v>8622522232.32</v>
       </c>
       <c r="E50" t="n">
         <v>7.10699987411499</v>
+      </c>
+      <c r="F50" t="n">
+        <v>4386713682.372519</v>
+      </c>
+      <c r="G50" t="n">
+        <v>1213243616.863541</v>
       </c>
     </row>
     <row r="51">
@@ -1278,13 +1564,19 @@
         <v>2024</v>
       </c>
       <c r="C51" t="n">
-        <v>4347921966.766748</v>
+        <v>31731569282.44</v>
       </c>
       <c r="D51" t="n">
-        <v>1265573896.468792</v>
+        <v>9236284847.059999</v>
       </c>
       <c r="E51" t="n">
         <v>7.298099994659424</v>
+      </c>
+      <c r="F51" t="n">
+        <v>4347921966.766748</v>
+      </c>
+      <c r="G51" t="n">
+        <v>1265573896.468792</v>
       </c>
     </row>
     <row r="52">
@@ -1295,13 +1587,19 @@
         <v>2015</v>
       </c>
       <c r="C52" t="n">
-        <v>4854634004.122005</v>
+        <v>31463854966.8</v>
       </c>
       <c r="D52" t="n">
-        <v>2010651488.055371</v>
+        <v>13031434863.11</v>
       </c>
       <c r="E52" t="n">
         <v>6.481200218200684</v>
+      </c>
+      <c r="F52" t="n">
+        <v>4854634004.122005</v>
+      </c>
+      <c r="G52" t="n">
+        <v>2010651488.055371</v>
       </c>
     </row>
     <row r="53">
@@ -1312,13 +1610,19 @@
         <v>2016</v>
       </c>
       <c r="C53" t="n">
-        <v>3355382949.442955</v>
+        <v>23304141541.8</v>
       </c>
       <c r="D53" t="n">
-        <v>2218013130.382258</v>
+        <v>15404766821.2</v>
       </c>
       <c r="E53" t="n">
         <v>6.945300102233887</v>
+      </c>
+      <c r="F53" t="n">
+        <v>3355382949.442955</v>
+      </c>
+      <c r="G53" t="n">
+        <v>2218013130.382258</v>
       </c>
     </row>
     <row r="54">
@@ -1329,13 +1633,19 @@
         <v>2017</v>
       </c>
       <c r="C54" t="n">
-        <v>5253584858.934463</v>
+        <v>34314314856.6</v>
       </c>
       <c r="D54" t="n">
-        <v>2658367633.233258</v>
+        <v>17363394029.17</v>
       </c>
       <c r="E54" t="n">
         <v>6.531599998474121</v>
+      </c>
+      <c r="F54" t="n">
+        <v>5253584858.934463</v>
+      </c>
+      <c r="G54" t="n">
+        <v>2658367633.233258</v>
       </c>
     </row>
     <row r="55">
@@ -1346,13 +1656,19 @@
         <v>2018</v>
       </c>
       <c r="C55" t="n">
-        <v>2847570502.437189</v>
+        <v>19583312220</v>
       </c>
       <c r="D55" t="n">
-        <v>2930174116.500823</v>
+        <v>20151393805.1</v>
       </c>
       <c r="E55" t="n">
         <v>6.877200126647949</v>
+      </c>
+      <c r="F55" t="n">
+        <v>2847570502.437189</v>
+      </c>
+      <c r="G55" t="n">
+        <v>2930174116.500823</v>
       </c>
     </row>
     <row r="56">
@@ -1363,13 +1679,19 @@
         <v>2019</v>
       </c>
       <c r="C56" t="n">
-        <v>5998520124.585538</v>
+        <v>41903862816.9</v>
       </c>
       <c r="D56" t="n">
-        <v>3136672193.207759</v>
+        <v>21911851349.31</v>
       </c>
       <c r="E56" t="n">
         <v>6.985700130462646</v>
+      </c>
+      <c r="F56" t="n">
+        <v>5998520124.585538</v>
+      </c>
+      <c r="G56" t="n">
+        <v>3136672193.207759</v>
       </c>
     </row>
     <row r="57">
@@ -1380,13 +1702,19 @@
         <v>2020</v>
       </c>
       <c r="C57" t="n">
-        <v>6551271060.337086</v>
+        <v>42728700814.48</v>
       </c>
       <c r="D57" t="n">
-        <v>4743567410.567491</v>
+        <v>30938495875.49</v>
       </c>
       <c r="E57" t="n">
         <v>6.522200107574463</v>
+      </c>
+      <c r="F57" t="n">
+        <v>6551271060.337086</v>
+      </c>
+      <c r="G57" t="n">
+        <v>4743567410.567491</v>
       </c>
     </row>
     <row r="58">
@@ -1397,13 +1725,19 @@
         <v>2021</v>
       </c>
       <c r="C58" t="n">
-        <v>5570436052.07148</v>
+        <v>35495374878.92</v>
       </c>
       <c r="D58" t="n">
-        <v>5627145556.300711</v>
+        <v>35856733503.81</v>
       </c>
       <c r="E58" t="n">
         <v>6.372099876403809</v>
+      </c>
+      <c r="F58" t="n">
+        <v>5570436052.07148</v>
+      </c>
+      <c r="G58" t="n">
+        <v>5627145556.300711</v>
       </c>
     </row>
     <row r="59">
@@ -1414,13 +1748,19 @@
         <v>2022</v>
       </c>
       <c r="C59" t="n">
-        <v>5136059956.261529</v>
+        <v>35762898858.09</v>
       </c>
       <c r="D59" t="n">
-        <v>5539840727.847381</v>
+        <v>38574464731.16</v>
       </c>
       <c r="E59" t="n">
         <v>6.963099956512451</v>
+      </c>
+      <c r="F59" t="n">
+        <v>5136059956.261529</v>
+      </c>
+      <c r="G59" t="n">
+        <v>5539840727.847381</v>
       </c>
     </row>
     <row r="60">
@@ -1431,13 +1771,19 @@
         <v>2023</v>
       </c>
       <c r="C60" t="n">
-        <v>4697811718.30084</v>
+        <v>33387347290.58</v>
       </c>
       <c r="D60" t="n">
-        <v>5530657604.458547</v>
+        <v>39306382898.66</v>
       </c>
       <c r="E60" t="n">
         <v>7.10699987411499</v>
+      </c>
+      <c r="F60" t="n">
+        <v>4697811718.30084</v>
+      </c>
+      <c r="G60" t="n">
+        <v>5530657604.458547</v>
       </c>
     </row>
     <row r="61">
@@ -1448,13 +1794,19 @@
         <v>2024</v>
       </c>
       <c r="C61" t="n">
-        <v>4952546788.266734</v>
+        <v>36144181689</v>
       </c>
       <c r="D61" t="n">
-        <v>5480608770.041465</v>
+        <v>39998030835.37</v>
       </c>
       <c r="E61" t="n">
         <v>7.298099994659424</v>
+      </c>
+      <c r="F61" t="n">
+        <v>4952546788.266734</v>
+      </c>
+      <c r="G61" t="n">
+        <v>5480608770.041465</v>
       </c>
     </row>
     <row r="62">
@@ -1469,6 +1821,8 @@
       <c r="E62" t="n">
         <v>6.481200218200684</v>
       </c>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -1482,6 +1836,8 @@
       <c r="E63" t="n">
         <v>6.945300102233887</v>
       </c>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -1495,6 +1851,8 @@
       <c r="E64" t="n">
         <v>6.531599998474121</v>
       </c>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -1508,6 +1866,8 @@
       <c r="E65" t="n">
         <v>6.877200126647949</v>
       </c>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -1518,10 +1878,14 @@
       </c>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="n">
-        <v>213699183.2930471</v>
+        <v>1492838412.61</v>
       </c>
       <c r="E66" t="n">
         <v>6.985700130462646</v>
+      </c>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="n">
+        <v>213699183.2930471</v>
       </c>
     </row>
     <row r="67">
@@ -1533,10 +1897,14 @@
       </c>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="n">
-        <v>201151232.1335231</v>
+        <v>1311948587.86</v>
       </c>
       <c r="E67" t="n">
         <v>6.522200107574463</v>
+      </c>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="n">
+        <v>201151232.1335231</v>
       </c>
     </row>
     <row r="68">
@@ -1548,10 +1916,14 @@
       </c>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="n">
-        <v>250244380.4082253</v>
+        <v>1594582185.47</v>
       </c>
       <c r="E68" t="n">
         <v>6.372099876403809</v>
+      </c>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="n">
+        <v>250244380.4082253</v>
       </c>
     </row>
     <row r="69">
@@ -1563,10 +1935,14 @@
       </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="n">
-        <v>275309165.1911535</v>
+        <v>1917005236.17</v>
       </c>
       <c r="E69" t="n">
         <v>6.963099956512451</v>
+      </c>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="n">
+        <v>275309165.1911535</v>
       </c>
     </row>
     <row r="70">
@@ -1577,13 +1953,19 @@
         <v>2023</v>
       </c>
       <c r="C70" t="n">
-        <v>1420535131.240197</v>
+        <v>10095742998.9</v>
       </c>
       <c r="D70" t="n">
-        <v>361570822.883966</v>
+        <v>2569683792.72</v>
       </c>
       <c r="E70" t="n">
         <v>7.10699987411499</v>
+      </c>
+      <c r="F70" t="n">
+        <v>1420535131.240197</v>
+      </c>
+      <c r="G70" t="n">
+        <v>361570822.883966</v>
       </c>
     </row>
     <row r="71">
@@ -1594,13 +1976,19 @@
         <v>2024</v>
       </c>
       <c r="C71" t="n">
-        <v>2115434143.336983</v>
+        <v>15438649910.19</v>
       </c>
       <c r="D71" t="n">
-        <v>380087220.547798</v>
+        <v>2773914542.25</v>
       </c>
       <c r="E71" t="n">
         <v>7.298099994659424</v>
+      </c>
+      <c r="F71" t="n">
+        <v>2115434143.336983</v>
+      </c>
+      <c r="G71" t="n">
+        <v>380087220.547798</v>
       </c>
     </row>
     <row r="72">
@@ -1611,13 +1999,19 @@
         <v>2015</v>
       </c>
       <c r="C72" t="n">
-        <v>1455077388.597963</v>
+        <v>9430647888.48</v>
       </c>
       <c r="D72" t="n">
-        <v>215653713.3916886</v>
+        <v>1397694894.29</v>
       </c>
       <c r="E72" t="n">
         <v>6.481200218200684</v>
+      </c>
+      <c r="F72" t="n">
+        <v>1455077388.597963</v>
+      </c>
+      <c r="G72" t="n">
+        <v>215653713.3916886</v>
       </c>
     </row>
     <row r="73">
@@ -1628,13 +2022,19 @@
         <v>2016</v>
       </c>
       <c r="C73" t="n">
-        <v>1224404978.046207</v>
+        <v>8503860019.2</v>
       </c>
       <c r="D73" t="n">
-        <v>230225098.4929655</v>
+        <v>1598982400.1</v>
       </c>
       <c r="E73" t="n">
         <v>6.945300102233887</v>
+      </c>
+      <c r="F73" t="n">
+        <v>1224404978.046207</v>
+      </c>
+      <c r="G73" t="n">
+        <v>230225098.4929655</v>
       </c>
     </row>
     <row r="74">
@@ -1645,13 +2045,19 @@
         <v>2017</v>
       </c>
       <c r="C74" t="n">
-        <v>1187605339.612368</v>
+        <v>7756963034.4</v>
       </c>
       <c r="D74" t="n">
-        <v>321907262.5805609</v>
+        <v>2102569475.78</v>
       </c>
       <c r="E74" t="n">
         <v>6.531599998474121</v>
+      </c>
+      <c r="F74" t="n">
+        <v>1187605339.612368</v>
+      </c>
+      <c r="G74" t="n">
+        <v>321907262.5805609</v>
       </c>
     </row>
     <row r="75">
@@ -1662,13 +2068,19 @@
         <v>2018</v>
       </c>
       <c r="C75" t="n">
-        <v>769000210.8252922</v>
+        <v>5288568347.28</v>
       </c>
       <c r="D75" t="n">
-        <v>526300221.0427436</v>
+        <v>3619471946.81</v>
       </c>
       <c r="E75" t="n">
         <v>6.877200126647949</v>
+      </c>
+      <c r="F75" t="n">
+        <v>769000210.8252922</v>
+      </c>
+      <c r="G75" t="n">
+        <v>526300221.0427436</v>
       </c>
     </row>
     <row r="76">
@@ -1679,13 +2091,19 @@
         <v>2019</v>
       </c>
       <c r="C76" t="n">
-        <v>1614400915.252728</v>
+        <v>11277720684.3</v>
       </c>
       <c r="D76" t="n">
-        <v>650276494.2472776</v>
+        <v>4542636590.7</v>
       </c>
       <c r="E76" t="n">
         <v>6.985700130462646</v>
+      </c>
+      <c r="F76" t="n">
+        <v>1614400915.252728</v>
+      </c>
+      <c r="G76" t="n">
+        <v>650276494.2472776</v>
       </c>
     </row>
     <row r="77">
@@ -1696,13 +2114,19 @@
         <v>2020</v>
       </c>
       <c r="C77" t="n">
-        <v>2420206691.945596</v>
+        <v>15785072346.56</v>
       </c>
       <c r="D77" t="n">
-        <v>949858725.5664434</v>
+        <v>6195168682.07</v>
       </c>
       <c r="E77" t="n">
         <v>6.522200107574463</v>
+      </c>
+      <c r="F77" t="n">
+        <v>2420206691.945596</v>
+      </c>
+      <c r="G77" t="n">
+        <v>949858725.5664434</v>
       </c>
     </row>
     <row r="78">
@@ -1713,13 +2137,19 @@
         <v>2021</v>
       </c>
       <c r="C78" t="n">
-        <v>3934571777.1752</v>
+        <v>25071484335.04</v>
       </c>
       <c r="D78" t="n">
-        <v>1120911470.29086</v>
+        <v>7142559841.3</v>
       </c>
       <c r="E78" t="n">
         <v>6.372099876403809</v>
+      </c>
+      <c r="F78" t="n">
+        <v>3934571777.1752</v>
+      </c>
+      <c r="G78" t="n">
+        <v>1120911470.29086</v>
       </c>
     </row>
     <row r="79">
@@ -1730,13 +2160,19 @@
         <v>2022</v>
       </c>
       <c r="C79" t="n">
-        <v>1914533364.529931</v>
+        <v>13331087187.3</v>
       </c>
       <c r="D79" t="n">
-        <v>1219380745.337261</v>
+        <v>8490670014.83</v>
       </c>
       <c r="E79" t="n">
         <v>6.963099956512451</v>
+      </c>
+      <c r="F79" t="n">
+        <v>1914533364.529931</v>
+      </c>
+      <c r="G79" t="n">
+        <v>1219380745.337261</v>
       </c>
     </row>
     <row r="80">
@@ -1747,13 +2183,19 @@
         <v>2023</v>
       </c>
       <c r="C80" t="n">
-        <v>1873766853.036325</v>
+        <v>13316860788.65</v>
       </c>
       <c r="D80" t="n">
-        <v>1402094499.440366</v>
+        <v>9964685431.02</v>
       </c>
       <c r="E80" t="n">
         <v>7.10699987411499</v>
+      </c>
+      <c r="F80" t="n">
+        <v>1873766853.036325</v>
+      </c>
+      <c r="G80" t="n">
+        <v>1402094499.440366</v>
       </c>
     </row>
     <row r="81">
@@ -1764,13 +2206,19 @@
         <v>2024</v>
       </c>
       <c r="C81" t="n">
-        <v>2295834846.55062</v>
+        <v>16755232281.35</v>
       </c>
       <c r="D81" t="n">
-        <v>1640228902.218354</v>
+        <v>11970554542.52</v>
       </c>
       <c r="E81" t="n">
         <v>7.298099994659424</v>
+      </c>
+      <c r="F81" t="n">
+        <v>2295834846.55062</v>
+      </c>
+      <c r="G81" t="n">
+        <v>1640228902.218354</v>
       </c>
     </row>
     <row r="82">
@@ -1785,6 +2233,8 @@
       <c r="E82" t="n">
         <v>6.481200218200684</v>
       </c>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -1795,10 +2245,14 @@
       </c>
       <c r="C83" t="inlineStr"/>
       <c r="D83" t="n">
-        <v>22704784.31583973</v>
+        <v>157691540.83</v>
       </c>
       <c r="E83" t="n">
         <v>6.945300102233887</v>
+      </c>
+      <c r="F83" t="inlineStr"/>
+      <c r="G83" t="n">
+        <v>22704784.31583973</v>
       </c>
     </row>
     <row r="84">
@@ -1810,10 +2264,14 @@
       </c>
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="n">
-        <v>41563536.31168793</v>
+        <v>271476393.71</v>
       </c>
       <c r="E84" t="n">
         <v>6.531599998474121</v>
+      </c>
+      <c r="F84" t="inlineStr"/>
+      <c r="G84" t="n">
+        <v>41563536.31168793</v>
       </c>
     </row>
     <row r="85">
@@ -1825,10 +2283,14 @@
       </c>
       <c r="C85" t="inlineStr"/>
       <c r="D85" t="n">
-        <v>53227115.76643037</v>
+        <v>366053527.29</v>
       </c>
       <c r="E85" t="n">
         <v>6.877200126647949</v>
+      </c>
+      <c r="F85" t="inlineStr"/>
+      <c r="G85" t="n">
+        <v>53227115.76643037</v>
       </c>
     </row>
     <row r="86">
@@ -1839,13 +2301,19 @@
         <v>2019</v>
       </c>
       <c r="C86" t="n">
-        <v>2250597607.452522</v>
+        <v>15722000000</v>
       </c>
       <c r="D86" t="n">
-        <v>317895441.8306711</v>
+        <v>2220722229.47</v>
       </c>
       <c r="E86" t="n">
         <v>6.985700130462646</v>
+      </c>
+      <c r="F86" t="n">
+        <v>2250597607.452522</v>
+      </c>
+      <c r="G86" t="n">
+        <v>317895441.8306711</v>
       </c>
     </row>
     <row r="87">
@@ -1856,13 +2324,19 @@
         <v>2020</v>
       </c>
       <c r="C87" t="n">
-        <v>4041887639.936848</v>
+        <v>26362000000</v>
       </c>
       <c r="D87" t="n">
-        <v>400391672.4047225</v>
+        <v>2611434608.83</v>
       </c>
       <c r="E87" t="n">
         <v>6.522200107574463</v>
+      </c>
+      <c r="F87" t="n">
+        <v>4041887639.936848</v>
+      </c>
+      <c r="G87" t="n">
+        <v>400391672.4047225</v>
       </c>
     </row>
     <row r="88">
@@ -1873,13 +2347,19 @@
         <v>2021</v>
       </c>
       <c r="C88" t="n">
-        <v>6069468908.815498</v>
+        <v>38675262083.7</v>
       </c>
       <c r="D88" t="n">
-        <v>494122447.4477257</v>
+        <v>3148597586.31</v>
       </c>
       <c r="E88" t="n">
         <v>6.372099876403809</v>
+      </c>
+      <c r="F88" t="n">
+        <v>6069468908.815498</v>
+      </c>
+      <c r="G88" t="n">
+        <v>494122447.4477257</v>
       </c>
     </row>
     <row r="89">
@@ -1890,13 +2370,19 @@
         <v>2022</v>
       </c>
       <c r="C89" t="n">
-        <v>4550875953.943852</v>
+        <v>31688204157</v>
       </c>
       <c r="D89" t="n">
-        <v>646953904.041941</v>
+        <v>4504804701.1</v>
       </c>
       <c r="E89" t="n">
         <v>6.963099956512451</v>
+      </c>
+      <c r="F89" t="n">
+        <v>4550875953.943852</v>
+      </c>
+      <c r="G89" t="n">
+        <v>646953904.041941</v>
       </c>
     </row>
     <row r="90">
@@ -1907,13 +2393,19 @@
         <v>2023</v>
       </c>
       <c r="C90" t="n">
-        <v>5211568255.958677</v>
+        <v>37038614939.04</v>
       </c>
       <c r="D90" t="n">
-        <v>750638985.2137605</v>
+        <v>5334791173.42</v>
       </c>
       <c r="E90" t="n">
         <v>7.10699987411499</v>
+      </c>
+      <c r="F90" t="n">
+        <v>5211568255.958677</v>
+      </c>
+      <c r="G90" t="n">
+        <v>750638985.2137605</v>
       </c>
     </row>
     <row r="91">
@@ -1924,13 +2416,19 @@
         <v>2024</v>
       </c>
       <c r="C91" t="n">
-        <v>5468435422.672284</v>
+        <v>39909188529</v>
       </c>
       <c r="D91" t="n">
-        <v>805408139.2172407</v>
+        <v>5877949136.52</v>
       </c>
       <c r="E91" t="n">
         <v>7.298099994659424</v>
+      </c>
+      <c r="F91" t="n">
+        <v>5468435422.672284</v>
+      </c>
+      <c r="G91" t="n">
+        <v>805408139.2172407</v>
       </c>
     </row>
     <row r="92">
@@ -1941,13 +2439,19 @@
         <v>2015</v>
       </c>
       <c r="C92" t="n">
-        <v>2092888228.113676</v>
+        <v>13564427640.72</v>
       </c>
       <c r="D92" t="n">
-        <v>1459959279.029483</v>
+        <v>9462288397.809999</v>
       </c>
       <c r="E92" t="n">
         <v>6.481200218200684</v>
+      </c>
+      <c r="F92" t="n">
+        <v>2092888228.113676</v>
+      </c>
+      <c r="G92" t="n">
+        <v>1459959279.029483</v>
       </c>
     </row>
     <row r="93">
@@ -1958,13 +2462,19 @@
         <v>2016</v>
       </c>
       <c r="C93" t="n">
-        <v>1453716814.216935</v>
+        <v>10096499538.4</v>
       </c>
       <c r="D93" t="n">
-        <v>1520024136.872709</v>
+        <v>10557023793.22</v>
       </c>
       <c r="E93" t="n">
         <v>6.945300102233887</v>
+      </c>
+      <c r="F93" t="n">
+        <v>1453716814.216935</v>
+      </c>
+      <c r="G93" t="n">
+        <v>1520024136.872709</v>
       </c>
     </row>
     <row r="94">
@@ -1975,13 +2485,19 @@
         <v>2017</v>
       </c>
       <c r="C94" t="n">
-        <v>1223192477.253115</v>
+        <v>7989403982.56</v>
       </c>
       <c r="D94" t="n">
-        <v>1704291745.941353</v>
+        <v>11131751965.19</v>
       </c>
       <c r="E94" t="n">
         <v>6.531599998474121</v>
+      </c>
+      <c r="F94" t="n">
+        <v>1223192477.253115</v>
+      </c>
+      <c r="G94" t="n">
+        <v>1704291745.941353</v>
       </c>
     </row>
     <row r="95">
@@ -1992,13 +2508,19 @@
         <v>2018</v>
       </c>
       <c r="C95" t="n">
-        <v>804270012.828019</v>
+        <v>5531125834.08</v>
       </c>
       <c r="D95" t="n">
-        <v>1604059382.962422</v>
+        <v>11031437391.66</v>
       </c>
       <c r="E95" t="n">
         <v>6.877200126647949</v>
+      </c>
+      <c r="F95" t="n">
+        <v>804270012.828019</v>
+      </c>
+      <c r="G95" t="n">
+        <v>1604059382.962422</v>
       </c>
     </row>
     <row r="96">
@@ -2009,13 +2531,19 @@
         <v>2019</v>
       </c>
       <c r="C96" t="n">
-        <v>1149963734.001272</v>
+        <v>8033301806.64</v>
       </c>
       <c r="D96" t="n">
-        <v>1427355506.081484</v>
+        <v>9971077545.049999</v>
       </c>
       <c r="E96" t="n">
         <v>6.985700130462646</v>
+      </c>
+      <c r="F96" t="n">
+        <v>1149963734.001272</v>
+      </c>
+      <c r="G96" t="n">
+        <v>1427355506.081484</v>
       </c>
     </row>
     <row r="97">
@@ -2026,13 +2554,19 @@
         <v>2020</v>
       </c>
       <c r="C97" t="n">
-        <v>1336009005.574737</v>
+        <v>8713718079.879999</v>
       </c>
       <c r="D97" t="n">
-        <v>1377818903.212393</v>
+        <v>8986410598.75</v>
       </c>
       <c r="E97" t="n">
         <v>6.522200107574463</v>
+      </c>
+      <c r="F97" t="n">
+        <v>1336009005.574737</v>
+      </c>
+      <c r="G97" t="n">
+        <v>1377818903.212393</v>
       </c>
     </row>
     <row r="98">
@@ -2043,13 +2577,19 @@
         <v>2021</v>
       </c>
       <c r="C98" t="n">
-        <v>837021661.4887855</v>
+        <v>5333585625.72</v>
       </c>
       <c r="D98" t="n">
-        <v>1279367461.708847</v>
+        <v>8152257244.63</v>
       </c>
       <c r="E98" t="n">
         <v>6.372099876403809</v>
+      </c>
+      <c r="F98" t="n">
+        <v>837021661.4887855</v>
+      </c>
+      <c r="G98" t="n">
+        <v>1279367461.708847</v>
       </c>
     </row>
     <row r="99">
@@ -2060,13 +2600,19 @@
         <v>2022</v>
       </c>
       <c r="C99" t="n">
-        <v>1575142021.988635</v>
+        <v>10967871344.81</v>
       </c>
       <c r="D99" t="n">
-        <v>827896696.3785093</v>
+        <v>5764727450.55</v>
       </c>
       <c r="E99" t="n">
         <v>6.963099956512451</v>
+      </c>
+      <c r="F99" t="n">
+        <v>1575142021.988635</v>
+      </c>
+      <c r="G99" t="n">
+        <v>827896696.3785093</v>
       </c>
     </row>
     <row r="100">
@@ -2077,13 +2623,19 @@
         <v>2023</v>
       </c>
       <c r="C100" t="n">
-        <v>1695813678.472987</v>
+        <v>12052147599.43</v>
       </c>
       <c r="D100" t="n">
-        <v>799953004.2327412</v>
+        <v>5685265900.38</v>
       </c>
       <c r="E100" t="n">
         <v>7.10699987411499</v>
+      </c>
+      <c r="F100" t="n">
+        <v>1695813678.472987</v>
+      </c>
+      <c r="G100" t="n">
+        <v>799953004.2327412</v>
       </c>
     </row>
     <row r="101">
@@ -2094,13 +2646,19 @@
         <v>2024</v>
       </c>
       <c r="C101" t="n">
-        <v>2508541612.656316</v>
+        <v>18307587529.93</v>
       </c>
       <c r="D101" t="n">
-        <v>968623193.6604055</v>
+        <v>7069108924.48</v>
       </c>
       <c r="E101" t="n">
         <v>7.298099994659424</v>
+      </c>
+      <c r="F101" t="n">
+        <v>2508541612.656316</v>
+      </c>
+      <c r="G101" t="n">
+        <v>968623193.6604055</v>
       </c>
     </row>
   </sheetData>

</xml_diff>